<commit_message>
Updated some functions and the xl
XL Is done
</commit_message>
<xml_diff>
--- a/Commands To Implement.xlsx
+++ b/Commands To Implement.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="148">
   <si>
     <t>DumpTelemetry</t>
   </si>
@@ -400,9 +400,6 @@
     <t>Shachar Sang</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>_ISISantsArmStatus</t>
   </si>
   <si>
@@ -473,6 +470,12 @@
   </si>
   <si>
     <t>Should check from telemtry if deployment is being initiated, No need</t>
+  </si>
+  <si>
+    <t>Maor</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -878,9 +881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +917,7 @@
         <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,10 +1093,10 @@
         <v>118</v>
       </c>
       <c r="F14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1113,7 +1116,7 @@
         <v>118</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,7 +1139,7 @@
         <v>120</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,7 +1181,7 @@
         <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -1190,10 +1193,10 @@
         <v>118</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
       </c>
       <c r="F21" s="5"/>
       <c r="H21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1240,7 +1243,7 @@
         <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -1252,15 +1255,15 @@
         <v>118</v>
       </c>
       <c r="F22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1279,19 +1282,19 @@
         <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1305,16 +1308,16 @@
         <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="G26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1324,11 +1327,14 @@
       <c r="B27" t="s">
         <v>52</v>
       </c>
+      <c r="D27" t="s">
+        <v>117</v>
+      </c>
       <c r="E27" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
       <c r="H27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1382,10 +1388,10 @@
         <v>118</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1402,7 +1408,7 @@
         <v>117</v>
       </c>
       <c r="E31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1419,7 +1425,7 @@
         <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,7 +1442,7 @@
         <v>117</v>
       </c>
       <c r="E33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,7 +1459,7 @@
         <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,7 +1476,7 @@
         <v>117</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,8 +1489,11 @@
       <c r="C36" t="s">
         <v>97</v>
       </c>
+      <c r="D36" t="s">
+        <v>117</v>
+      </c>
       <c r="E36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1497,8 +1506,11 @@
       <c r="C37" t="s">
         <v>97</v>
       </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
       <c r="E37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1511,8 +1523,11 @@
       <c r="C38" t="s">
         <v>97</v>
       </c>
+      <c r="D38" t="s">
+        <v>117</v>
+      </c>
       <c r="E38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1525,8 +1540,11 @@
       <c r="C39" t="s">
         <v>97</v>
       </c>
+      <c r="D39" t="s">
+        <v>117</v>
+      </c>
       <c r="E39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,8 +1557,11 @@
       <c r="C40" t="s">
         <v>97</v>
       </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
       <c r="E40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1553,8 +1574,11 @@
       <c r="C41" t="s">
         <v>97</v>
       </c>
+      <c r="D41" t="s">
+        <v>117</v>
+      </c>
       <c r="E41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1567,8 +1591,11 @@
       <c r="C42" t="s">
         <v>97</v>
       </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
       <c r="E42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1581,8 +1608,11 @@
       <c r="C43" t="s">
         <v>97</v>
       </c>
+      <c r="D43" t="s">
+        <v>117</v>
+      </c>
       <c r="E43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1595,8 +1625,11 @@
       <c r="C44" t="s">
         <v>97</v>
       </c>
+      <c r="D44" t="s">
+        <v>117</v>
+      </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1609,8 +1642,11 @@
       <c r="C45" t="s">
         <v>97</v>
       </c>
+      <c r="D45" t="s">
+        <v>147</v>
+      </c>
       <c r="E45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1623,8 +1659,11 @@
       <c r="C46" t="s">
         <v>97</v>
       </c>
+      <c r="D46" t="s">
+        <v>117</v>
+      </c>
       <c r="E46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1637,16 +1676,22 @@
       <c r="C47" t="s">
         <v>97</v>
       </c>
+      <c r="D47" t="s">
+        <v>117</v>
+      </c>
       <c r="E47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
+      <c r="D48" t="s">
+        <v>117</v>
+      </c>
       <c r="E48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1659,6 +1704,9 @@
       <c r="C49" t="s">
         <v>96</v>
       </c>
+      <c r="D49" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1670,6 +1718,9 @@
       <c r="C50" t="s">
         <v>96</v>
       </c>
+      <c r="D50" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -1681,6 +1732,9 @@
       <c r="C51" t="s">
         <v>96</v>
       </c>
+      <c r="D51" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1698,7 +1752,7 @@
         <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1712,7 +1766,7 @@
         <v>117</v>
       </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,13 +1777,13 @@
         <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,13 +1794,13 @@
         <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D57" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1763,7 +1817,7 @@
         <v>117</v>
       </c>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,7 +1834,7 @@
         <v>117</v>
       </c>
       <c r="E59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Copied what we dont have
</commit_message>
<xml_diff>
--- a/Commands To Implement.xlsx
+++ b/Commands To Implement.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
   <si>
     <t>DumpTelemetry</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Command Name</t>
   </si>
   <si>
-    <t>Method source</t>
-  </si>
-  <si>
     <t>TRXVU.c</t>
   </si>
   <si>
@@ -82,21 +79,12 @@
     <t>Ido</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Programmer Notes</t>
   </si>
   <si>
     <t>InitSemaphores</t>
   </si>
   <si>
-    <t>GetNumberOfFramesInBuffer</t>
-  </si>
-  <si>
-    <t>CheckTransmitionAllowed</t>
-  </si>
-  <si>
     <t>FinishDump</t>
   </si>
   <si>
@@ -106,18 +94,6 @@
     <t>DumpTask</t>
   </si>
   <si>
-    <t>BeaconSetBitrate</t>
-  </si>
-  <si>
-    <t>TransmitDataAsSPL_Packet</t>
-  </si>
-  <si>
-    <t>UpdateBeaconBaudCycle</t>
-  </si>
-  <si>
-    <t>UpdateBeaconInterval</t>
-  </si>
-  <si>
     <t>isDelayedCommandDue</t>
   </si>
   <si>
@@ -226,19 +202,13 @@
     <t>Problem</t>
   </si>
   <si>
-    <t>No Subtypes</t>
-  </si>
-  <si>
-    <t>what to write and how to transmit</t>
-  </si>
-  <si>
-    <t>what to read and how to transmit</t>
-  </si>
-  <si>
-    <t>HOW?</t>
-  </si>
-  <si>
-    <t>HOW???</t>
+    <t>They didn’t do anything in here so I left it empty</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Empty</t>
   </si>
 </sst>
 </file>
@@ -290,12 +260,12 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,20 +581,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1"/>
     <col min="8" max="8" width="39.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -634,356 +605,540 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
+      <c r="A12" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="4"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>8</v>
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>64</v>
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="D36" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="D37" t="s">
-        <v>14</v>
-      </c>
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>62</v>
+      <c r="C56" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>